<commit_message>
extend facility report to all container types, 705
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/facility_tank_template.xlsx
+++ b/bio_diversity/static/report_templates/facility_tank_template.xlsx
@@ -21,16 +21,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Tank Name:</t>
+    <t>Collection</t>
   </si>
   <si>
-    <t>Taged Fish in Tank</t>
+    <t>Container Name:</t>
   </si>
   <si>
-    <t># of Fish in tank</t>
+    <t>Taged Fish in Container</t>
   </si>
   <si>
-    <t>Collection</t>
+    <t># of Fish in Container</t>
   </si>
 </sst>
 </file>
@@ -872,7 +872,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,16 +906,16 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add feeding to facility report
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/facility_tank_template.xlsx
+++ b/bio_diversity/static/report_templates/facility_tank_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Collection</t>
   </si>
@@ -32,6 +32,9 @@
   <si>
     <t># of Fish in Container</t>
   </si>
+  <si>
+    <t>Feed</t>
+  </si>
 </sst>
 </file>
 
@@ -177,7 +180,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,8 +360,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -470,6 +479,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -518,12 +536,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -872,14 +892,16 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -904,18 +926,21 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>0</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start updating datetimes, add date to facility tank report
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/facility_tank_template.xlsx
+++ b/bio_diversity/static/report_templates/facility_tank_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Collection</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Feed</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -892,7 +895,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,6 +905,7 @@
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -942,6 +946,9 @@
       <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="F2" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>